<commit_message>
Advanced lesson on pandas function added
</commit_message>
<xml_diff>
--- a/data/test/ad_campaigns.xlsx
+++ b/data/test/ad_campaigns.xlsx
@@ -8003,7 +8003,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -8420,7 +8420,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -8445,7 +8445,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -8470,7 +8470,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -8495,7 +8495,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -8520,7 +8520,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -8545,7 +8545,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -8570,7 +8570,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -8595,7 +8595,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -8620,7 +8620,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -8645,7 +8645,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
@@ -8670,7 +8670,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
@@ -8695,7 +8695,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -8720,7 +8720,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -8745,7 +8745,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
@@ -8770,7 +8770,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
@@ -8795,7 +8795,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
@@ -8820,7 +8820,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4" t="s">
         <v>45</v>
       </c>
@@ -8845,7 +8845,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4" t="s">
         <v>45</v>
       </c>
@@ -8870,7 +8870,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4" t="s">
         <v>45</v>
       </c>
@@ -8895,7 +8895,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4" t="s">
         <v>49</v>
       </c>
@@ -8920,7 +8920,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4" t="s">
         <v>49</v>
       </c>
@@ -8945,7 +8945,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="4" t="s">
         <v>49</v>
       </c>
@@ -8970,7 +8970,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4" t="s">
         <v>53</v>
       </c>
@@ -8995,7 +8995,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="4" t="s">
         <v>53</v>
       </c>
@@ -9020,7 +9020,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="4" t="s">
         <v>53</v>
       </c>
@@ -9045,7 +9045,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -9070,7 +9070,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="4" t="s">
         <v>57</v>
       </c>
@@ -9095,7 +9095,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="4" t="s">
         <v>57</v>
       </c>
@@ -9120,7 +9120,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="4" t="s">
         <v>61</v>
       </c>
@@ -9145,7 +9145,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
@@ -9170,7 +9170,7 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="4" t="s">
         <v>61</v>
       </c>
@@ -9195,7 +9195,7 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="4" t="s">
         <v>65</v>
       </c>

</xml_diff>